<commit_message>
adding border and increaments
</commit_message>
<xml_diff>
--- a/tagged.xlsx
+++ b/tagged.xlsx
@@ -524,102 +524,256 @@
       </c>
     </row>
     <row r="4">
+      <c r="A4" s="2" t="n">
+        <v>1</v>
+      </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
           <t>20221218133806_Full.png</t>
         </is>
       </c>
+      <c r="C4" s="2" t="n"/>
+      <c r="D4" s="2" t="n"/>
+      <c r="E4" s="2" t="n"/>
+      <c r="F4" s="2" t="n"/>
+      <c r="G4" s="2" t="n"/>
+      <c r="H4" s="2" t="n"/>
+      <c r="I4" s="2" t="n"/>
+      <c r="J4" s="2" t="n"/>
     </row>
     <row r="5">
-      <c r="B5" t="inlineStr">
+      <c r="A5" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
         <is>
           <t>20221218133816_Full.png</t>
         </is>
       </c>
+      <c r="C5" s="2" t="n"/>
+      <c r="D5" s="2" t="n"/>
+      <c r="E5" s="2" t="n"/>
+      <c r="F5" s="2" t="n"/>
+      <c r="G5" s="2" t="n"/>
+      <c r="H5" s="2" t="n"/>
+      <c r="I5" s="2" t="n"/>
+      <c r="J5" s="2" t="n"/>
     </row>
     <row r="6">
-      <c r="B6" t="inlineStr">
+      <c r="A6" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
         <is>
           <t>20221218133825_Full.png</t>
         </is>
       </c>
+      <c r="C6" s="2" t="n"/>
+      <c r="D6" s="2" t="n"/>
+      <c r="E6" s="2" t="n"/>
+      <c r="F6" s="2" t="n"/>
+      <c r="G6" s="2" t="n"/>
+      <c r="H6" s="2" t="n"/>
+      <c r="I6" s="2" t="n"/>
+      <c r="J6" s="2" t="n"/>
     </row>
     <row r="7">
-      <c r="B7" t="inlineStr">
+      <c r="A7" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
         <is>
           <t>20221218133829_Full.png</t>
         </is>
       </c>
+      <c r="C7" s="2" t="n"/>
+      <c r="D7" s="2" t="n"/>
+      <c r="E7" s="2" t="n"/>
+      <c r="F7" s="2" t="n"/>
+      <c r="G7" s="2" t="n"/>
+      <c r="H7" s="2" t="n"/>
+      <c r="I7" s="2" t="n"/>
+      <c r="J7" s="2" t="n"/>
     </row>
     <row r="8">
-      <c r="B8" t="inlineStr">
+      <c r="A8" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
         <is>
           <t>20221218133834_Full.png</t>
         </is>
       </c>
+      <c r="C8" s="2" t="n"/>
+      <c r="D8" s="2" t="n"/>
+      <c r="E8" s="2" t="n"/>
+      <c r="F8" s="2" t="n"/>
+      <c r="G8" s="2" t="n"/>
+      <c r="H8" s="2" t="n"/>
+      <c r="I8" s="2" t="n"/>
+      <c r="J8" s="2" t="n"/>
     </row>
     <row r="9">
-      <c r="B9" t="inlineStr">
+      <c r="A9" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="inlineStr">
         <is>
           <t>20221218133839_Full.png</t>
         </is>
       </c>
+      <c r="C9" s="2" t="n"/>
+      <c r="D9" s="2" t="n"/>
+      <c r="E9" s="2" t="n"/>
+      <c r="F9" s="2" t="n"/>
+      <c r="G9" s="2" t="n"/>
+      <c r="H9" s="2" t="n"/>
+      <c r="I9" s="2" t="n"/>
+      <c r="J9" s="2" t="n"/>
     </row>
     <row r="10">
-      <c r="B10" t="inlineStr">
+      <c r="A10" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="B10" s="2" t="inlineStr">
         <is>
           <t>20221218133845_Full.png</t>
         </is>
       </c>
+      <c r="C10" s="2" t="n"/>
+      <c r="D10" s="2" t="n"/>
+      <c r="E10" s="2" t="n"/>
+      <c r="F10" s="2" t="n"/>
+      <c r="G10" s="2" t="n"/>
+      <c r="H10" s="2" t="n"/>
+      <c r="I10" s="2" t="n"/>
+      <c r="J10" s="2" t="n"/>
     </row>
     <row r="11">
-      <c r="B11" t="inlineStr">
+      <c r="A11" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="B11" s="2" t="inlineStr">
         <is>
           <t>20221218133851_Full.png</t>
         </is>
       </c>
+      <c r="C11" s="2" t="n"/>
+      <c r="D11" s="2" t="n"/>
+      <c r="E11" s="2" t="n"/>
+      <c r="F11" s="2" t="n"/>
+      <c r="G11" s="2" t="n"/>
+      <c r="H11" s="2" t="n"/>
+      <c r="I11" s="2" t="n"/>
+      <c r="J11" s="2" t="n"/>
     </row>
     <row r="12">
-      <c r="B12" t="inlineStr">
+      <c r="A12" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="B12" s="2" t="inlineStr">
         <is>
           <t>20221218133856_Full.png</t>
         </is>
       </c>
+      <c r="C12" s="2" t="n"/>
+      <c r="D12" s="2" t="n"/>
+      <c r="E12" s="2" t="n"/>
+      <c r="F12" s="2" t="n"/>
+      <c r="G12" s="2" t="n"/>
+      <c r="H12" s="2" t="n"/>
+      <c r="I12" s="2" t="n"/>
+      <c r="J12" s="2" t="n"/>
     </row>
     <row r="13">
-      <c r="B13" t="inlineStr">
+      <c r="A13" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="B13" s="2" t="inlineStr">
         <is>
           <t>20221218133901_Full.png</t>
         </is>
       </c>
+      <c r="C13" s="2" t="n"/>
+      <c r="D13" s="2" t="n"/>
+      <c r="E13" s="2" t="n"/>
+      <c r="F13" s="2" t="n"/>
+      <c r="G13" s="2" t="n"/>
+      <c r="H13" s="2" t="n"/>
+      <c r="I13" s="2" t="n"/>
+      <c r="J13" s="2" t="n"/>
     </row>
     <row r="14">
-      <c r="B14" t="inlineStr">
+      <c r="A14" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="B14" s="2" t="inlineStr">
         <is>
           <t>20221218133905_Full.png</t>
         </is>
       </c>
+      <c r="C14" s="2" t="n"/>
+      <c r="D14" s="2" t="n"/>
+      <c r="E14" s="2" t="n"/>
+      <c r="F14" s="2" t="n"/>
+      <c r="G14" s="2" t="n"/>
+      <c r="H14" s="2" t="n"/>
+      <c r="I14" s="2" t="n"/>
+      <c r="J14" s="2" t="n"/>
     </row>
     <row r="15">
-      <c r="B15" t="inlineStr">
+      <c r="A15" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="B15" s="2" t="inlineStr">
         <is>
           <t>20221218133910_Full.png</t>
         </is>
       </c>
+      <c r="C15" s="2" t="n"/>
+      <c r="D15" s="2" t="n"/>
+      <c r="E15" s="2" t="n"/>
+      <c r="F15" s="2" t="n"/>
+      <c r="G15" s="2" t="n"/>
+      <c r="H15" s="2" t="n"/>
+      <c r="I15" s="2" t="n"/>
+      <c r="J15" s="2" t="n"/>
     </row>
     <row r="16">
-      <c r="B16" t="inlineStr">
+      <c r="A16" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="B16" s="2" t="inlineStr">
         <is>
           <t>20221218133921_Full.png</t>
         </is>
       </c>
+      <c r="C16" s="2" t="n"/>
+      <c r="D16" s="2" t="n"/>
+      <c r="E16" s="2" t="n"/>
+      <c r="F16" s="2" t="n"/>
+      <c r="G16" s="2" t="n"/>
+      <c r="H16" s="2" t="n"/>
+      <c r="I16" s="2" t="n"/>
+      <c r="J16" s="2" t="n"/>
     </row>
     <row r="17">
-      <c r="B17" t="inlineStr">
+      <c r="A17" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="B17" s="2" t="inlineStr">
         <is>
           <t>20221218133927_Full.png</t>
         </is>
       </c>
+      <c r="C17" s="2" t="n"/>
+      <c r="D17" s="2" t="n"/>
+      <c r="E17" s="2" t="n"/>
+      <c r="F17" s="2" t="n"/>
+      <c r="G17" s="2" t="n"/>
+      <c r="H17" s="2" t="n"/>
+      <c r="I17" s="2" t="n"/>
+      <c r="J17" s="2" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
adding auto Define Time (PAGI/MALAM)
</commit_message>
<xml_diff>
--- a/tagged.xlsx
+++ b/tagged.xlsx
@@ -539,7 +539,11 @@
       <c r="G4" s="2" t="n"/>
       <c r="H4" s="2" t="n"/>
       <c r="I4" s="2" t="n"/>
-      <c r="J4" s="2" t="n"/>
+      <c r="J4" s="2" t="inlineStr">
+        <is>
+          <t>PAGI</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
@@ -557,7 +561,11 @@
       <c r="G5" s="2" t="n"/>
       <c r="H5" s="2" t="n"/>
       <c r="I5" s="2" t="n"/>
-      <c r="J5" s="2" t="n"/>
+      <c r="J5" s="2" t="inlineStr">
+        <is>
+          <t>PAGI</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
@@ -575,7 +583,11 @@
       <c r="G6" s="2" t="n"/>
       <c r="H6" s="2" t="n"/>
       <c r="I6" s="2" t="n"/>
-      <c r="J6" s="2" t="n"/>
+      <c r="J6" s="2" t="inlineStr">
+        <is>
+          <t>PAGI</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
@@ -593,7 +605,11 @@
       <c r="G7" s="2" t="n"/>
       <c r="H7" s="2" t="n"/>
       <c r="I7" s="2" t="n"/>
-      <c r="J7" s="2" t="n"/>
+      <c r="J7" s="2" t="inlineStr">
+        <is>
+          <t>PAGI</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
@@ -611,7 +627,11 @@
       <c r="G8" s="2" t="n"/>
       <c r="H8" s="2" t="n"/>
       <c r="I8" s="2" t="n"/>
-      <c r="J8" s="2" t="n"/>
+      <c r="J8" s="2" t="inlineStr">
+        <is>
+          <t>PAGI</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
@@ -629,7 +649,11 @@
       <c r="G9" s="2" t="n"/>
       <c r="H9" s="2" t="n"/>
       <c r="I9" s="2" t="n"/>
-      <c r="J9" s="2" t="n"/>
+      <c r="J9" s="2" t="inlineStr">
+        <is>
+          <t>PAGI</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
@@ -647,7 +671,11 @@
       <c r="G10" s="2" t="n"/>
       <c r="H10" s="2" t="n"/>
       <c r="I10" s="2" t="n"/>
-      <c r="J10" s="2" t="n"/>
+      <c r="J10" s="2" t="inlineStr">
+        <is>
+          <t>PAGI</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
@@ -665,7 +693,11 @@
       <c r="G11" s="2" t="n"/>
       <c r="H11" s="2" t="n"/>
       <c r="I11" s="2" t="n"/>
-      <c r="J11" s="2" t="n"/>
+      <c r="J11" s="2" t="inlineStr">
+        <is>
+          <t>PAGI</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
@@ -683,7 +715,11 @@
       <c r="G12" s="2" t="n"/>
       <c r="H12" s="2" t="n"/>
       <c r="I12" s="2" t="n"/>
-      <c r="J12" s="2" t="n"/>
+      <c r="J12" s="2" t="inlineStr">
+        <is>
+          <t>PAGI</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
@@ -701,7 +737,11 @@
       <c r="G13" s="2" t="n"/>
       <c r="H13" s="2" t="n"/>
       <c r="I13" s="2" t="n"/>
-      <c r="J13" s="2" t="n"/>
+      <c r="J13" s="2" t="inlineStr">
+        <is>
+          <t>PAGI</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
@@ -719,7 +759,11 @@
       <c r="G14" s="2" t="n"/>
       <c r="H14" s="2" t="n"/>
       <c r="I14" s="2" t="n"/>
-      <c r="J14" s="2" t="n"/>
+      <c r="J14" s="2" t="inlineStr">
+        <is>
+          <t>PAGI</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
@@ -737,7 +781,11 @@
       <c r="G15" s="2" t="n"/>
       <c r="H15" s="2" t="n"/>
       <c r="I15" s="2" t="n"/>
-      <c r="J15" s="2" t="n"/>
+      <c r="J15" s="2" t="inlineStr">
+        <is>
+          <t>PAGI</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
@@ -755,7 +803,11 @@
       <c r="G16" s="2" t="n"/>
       <c r="H16" s="2" t="n"/>
       <c r="I16" s="2" t="n"/>
-      <c r="J16" s="2" t="n"/>
+      <c r="J16" s="2" t="inlineStr">
+        <is>
+          <t>PAGI</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
@@ -773,7 +825,11 @@
       <c r="G17" s="2" t="n"/>
       <c r="H17" s="2" t="n"/>
       <c r="I17" s="2" t="n"/>
-      <c r="J17" s="2" t="n"/>
+      <c r="J17" s="2" t="inlineStr">
+        <is>
+          <t>PAGI</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>